<commit_message>
fix: correct handling of empty cells
Tests passes
</commit_message>
<xml_diff>
--- a/IntoRdf.Tests/TestData/emptycells.xlsx
+++ b/IntoRdf.Tests/TestData/emptycells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\toftalisk\esrc\into-rdf\IntoRdf.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230E1974-106C-4EC9-81D6-3AD43E9CF26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE45158-1994-4CD3-8846-1D0258FE5399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{C5BC0043-3F63-4953-A163-CADFB756E785}"/>
+    <workbookView xWindow="12390" yWindow="0" windowWidth="16515" windowHeight="15585" xr2:uid="{C5BC0043-3F63-4953-A163-CADFB756E785}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>a</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>noid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +445,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">

</xml_diff>